<commit_message>
Arreglo en GitHub Actions "parser" + results
</commit_message>
<xml_diff>
--- a/final_results/2/counting.xlsx
+++ b/final_results/2/counting.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -465,7 +465,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>212</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -478,7 +478,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -491,7 +491,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>6</v>
+        <v>495</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -504,7 +504,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -543,7 +543,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
@@ -569,7 +569,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
@@ -621,7 +621,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>7</v>
+        <v>669</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>

</xml_diff>